<commit_message>
updated some explanations, cleaned some graphs
</commit_message>
<xml_diff>
--- a/olympics.xlsx
+++ b/olympics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliajones/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliajones/Desktop/olympics_covid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC4E18B-E8BF-3D4A-A132-E1747D30F618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D1DD73-0310-6F45-B5AE-FAF9151A05CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8560" yWindow="500" windowWidth="20240" windowHeight="16360" xr2:uid="{967CFCA4-4CE2-D346-95F0-716D1DA2A879}"/>
+    <workbookView xWindow="8560" yWindow="500" windowWidth="20240" windowHeight="16360" xr2:uid="{967CFCA4-4CE2-D346-95F0-716D1DA2A879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>Bryson DeChambeau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US </t>
   </si>
   <si>
     <t>golf</t>
@@ -697,7 +694,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +737,7 @@
         <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -751,7 +748,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>44</v>
@@ -768,7 +765,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>44</v>
@@ -785,7 +782,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>44</v>
@@ -802,7 +799,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>44</v>
@@ -867,7 +864,7 @@
         <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -1074,7 +1071,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
@@ -1242,10 +1239,10 @@
         <v>60</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
@@ -1256,13 +1253,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
@@ -1271,18 +1268,18 @@
         <v>20</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>11</v>
@@ -1293,10 +1290,10 @@
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>12</v>
@@ -1310,7 +1307,7 @@
     </row>
     <row r="36" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>24</v>
@@ -1327,13 +1324,13 @@
     </row>
     <row r="37" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>11</v>
@@ -1342,18 +1339,18 @@
         <v>20</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>44</v>
@@ -1364,13 +1361,13 @@
     </row>
     <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>11</v>
@@ -1379,18 +1376,18 @@
         <v>20</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>11</v>
@@ -1399,18 +1396,18 @@
         <v>20</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="C41" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>44</v>
@@ -1421,13 +1418,13 @@
     </row>
     <row r="42" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>44</v>
@@ -1438,10 +1435,10 @@
     </row>
     <row r="43" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>43</v>
@@ -1455,13 +1452,13 @@
     </row>
     <row r="44" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="C44" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>11</v>
@@ -1472,7 +1469,7 @@
     </row>
     <row r="45" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>24</v>
@@ -1489,10 +1486,10 @@
     </row>
     <row r="46" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>12</v>
@@ -1506,13 +1503,13 @@
     </row>
     <row r="47" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>44</v>
@@ -1523,13 +1520,13 @@
     </row>
     <row r="48" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>44</v>
@@ -1540,13 +1537,13 @@
     </row>
     <row r="49" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>44</v>

</xml_diff>